<commit_message>
Ajout de quoi calculer les résultats.
</commit_message>
<xml_diff>
--- a/Docs/doc_synthese/optimal.xlsx
+++ b/Docs/doc_synthese/optimal.xlsx
@@ -15,7 +15,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="32">
+  <si>
+    <t>Erwan</t>
+  </si>
+  <si>
+    <t>Bichon</t>
+  </si>
   <si>
     <t>XML</t>
   </si>
@@ -42,6 +48,9 @@
   </si>
   <si>
     <t>a280</t>
+  </si>
+  <si>
+    <t>83.306</t>
   </si>
   <si>
     <t>att48</t>
@@ -226,17 +235,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.52549019607843"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.5843137254902"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.54509803921569"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.8588235294118"/>
+    <col collapsed="false" hidden="false" max="13" min="7" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.8588235294118"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -248,63 +259,98 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
-      <c r="A4" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="n">
-        <v>2579</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4" t="n">
-        <f aca="false">(D4-C4)/C4*100</f>
-        <v>-100</v>
+      <c r="F4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
       <c r="A5" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>10628</v>
+        <v>2579</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -312,16 +358,35 @@
         <f aca="false">(D5-C5)/C5*100</f>
         <v>-100</v>
       </c>
+      <c r="I5" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="4" t="n">
+        <v>2579</v>
+      </c>
+      <c r="L5" s="4" t="n">
+        <v>2825</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="4" t="n">
+        <f aca="false">(L5-K5)/K5*100</f>
+        <v>9.53858084528887</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="6">
       <c r="A6" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6" s="4" t="n">
-        <v>27686</v>
+        <v>10628</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -329,16 +394,31 @@
         <f aca="false">(D6-C6)/C6*100</f>
         <v>-100</v>
       </c>
+      <c r="I6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="4" t="n">
+        <v>10628</v>
+      </c>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4" t="n">
+        <f aca="false">(L6-K6)/K6*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7">
       <c r="A7" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C7" s="4" t="n">
-        <v>39</v>
+        <v>27686</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -346,16 +426,31 @@
         <f aca="false">(D7-C7)/C7*100</f>
         <v>-100</v>
       </c>
+      <c r="I7" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="4" t="n">
+        <v>27686</v>
+      </c>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4" t="n">
+        <f aca="false">(L7-K7)/K7*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="8">
       <c r="A8" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C8" s="4" t="n">
-        <v>25395</v>
+        <v>39</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -363,16 +458,31 @@
         <f aca="false">(D8-C8)/C8*100</f>
         <v>-100</v>
       </c>
+      <c r="I8" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4" t="n">
+        <f aca="false">(L8-K8)/K8*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="A9" s="4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C9" s="4" t="n">
-        <v>22204</v>
+        <v>25395</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -380,16 +490,31 @@
         <f aca="false">(D9-C9)/C9*100</f>
         <v>-100</v>
       </c>
+      <c r="I9" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="4" t="n">
+        <v>25395</v>
+      </c>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4" t="n">
+        <f aca="false">(L9-K9)/K9*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="10">
       <c r="A10" s="4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C10" s="4" t="n">
-        <v>28723</v>
+        <v>22204</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -397,16 +522,31 @@
         <f aca="false">(D10-C10)/C10*100</f>
         <v>-100</v>
       </c>
+      <c r="I10" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="4" t="n">
+        <v>22204</v>
+      </c>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4" t="n">
+        <f aca="false">(L10-K10)/K10*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="11">
       <c r="A11" s="4" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C11" s="4" t="n">
-        <v>182566</v>
+        <v>28723</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -414,16 +554,31 @@
         <f aca="false">(D11-C11)/C11*100</f>
         <v>-100</v>
       </c>
+      <c r="I11" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="4" t="n">
+        <v>28723</v>
+      </c>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4" t="n">
+        <f aca="false">(L11-K11)/K11*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="12">
       <c r="A12" s="4" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C12" s="4" t="n">
-        <v>22141</v>
+        <v>182566</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -431,16 +586,31 @@
         <f aca="false">(D12-C12)/C12*100</f>
         <v>-100</v>
       </c>
+      <c r="I12" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="4" t="n">
+        <v>182566</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4" t="n">
+        <f aca="false">(L12-K12)/K12*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="13">
       <c r="A13" s="4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C13" s="4" t="n">
-        <v>26130</v>
+        <v>22141</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -448,16 +618,31 @@
         <f aca="false">(D13-C13)/C13*100</f>
         <v>-100</v>
       </c>
+      <c r="I13" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="4" t="n">
+        <v>22141</v>
+      </c>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4" t="n">
+        <f aca="false">(L13-K13)/K13*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="14">
       <c r="A14" s="4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C14" s="4" t="n">
-        <v>29437</v>
+        <v>26130</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -465,16 +650,31 @@
         <f aca="false">(D14-C14)/C14*100</f>
         <v>-100</v>
       </c>
+      <c r="I14" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="4" t="n">
+        <v>26130</v>
+      </c>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4" t="n">
+        <f aca="false">(L14-K14)/K14*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="15">
       <c r="A15" s="4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C15" s="4" t="n">
-        <v>20749</v>
+        <v>29437</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -482,16 +682,31 @@
         <f aca="false">(D15-C15)/C15*100</f>
         <v>-100</v>
       </c>
+      <c r="I15" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" s="4" t="n">
+        <v>29437</v>
+      </c>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4" t="n">
+        <f aca="false">(L15-K15)/K15*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="16">
       <c r="A16" s="4" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C16" s="4" t="n">
-        <v>21294</v>
+        <v>20749</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -499,16 +714,31 @@
         <f aca="false">(D16-C16)/C16*100</f>
         <v>-100</v>
       </c>
+      <c r="I16" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" s="4" t="n">
+        <v>20749</v>
+      </c>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4" t="n">
+        <f aca="false">(L16-K16)/K16*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="17">
       <c r="A17" s="4" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C17" s="4" t="n">
-        <v>23260728</v>
+        <v>21294</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -516,16 +746,31 @@
         <f aca="false">(D17-C17)/C17*100</f>
         <v>-100</v>
       </c>
+      <c r="I17" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="4" t="n">
+        <v>21294</v>
+      </c>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4" t="n">
+        <f aca="false">(L17-K17)/K17*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="18">
       <c r="A18" s="4" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C18" s="4" t="n">
-        <v>378032</v>
+        <v>23260728</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -533,16 +778,31 @@
         <f aca="false">(D18-C18)/C18*100</f>
         <v>-100</v>
       </c>
+      <c r="I18" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="4" t="n">
+        <v>23260728</v>
+      </c>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4" t="n">
+        <f aca="false">(L18-K18)/K18*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="19">
       <c r="A19" s="4" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C19" s="4" t="n">
-        <v>565040</v>
+        <v>378032</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -550,16 +810,31 @@
         <f aca="false">(D19-C19)/C19*100</f>
         <v>-100</v>
       </c>
+      <c r="I19" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" s="4" t="n">
+        <v>378032</v>
+      </c>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4" t="n">
+        <f aca="false">(L19-K19)/K19*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="20">
       <c r="A20" s="4" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C20" s="4" t="n">
-        <v>554070</v>
+        <v>565040</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -567,16 +842,31 @@
         <f aca="false">(D20-C20)/C20*100</f>
         <v>-100</v>
       </c>
+      <c r="I20" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K20" s="4" t="n">
+        <v>565040</v>
+      </c>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4" t="n">
+        <f aca="false">(L20-K20)/K20*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="21">
       <c r="A21" s="4" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C21" s="4" t="n">
-        <v>224094</v>
+        <v>554070</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -584,16 +874,31 @@
         <f aca="false">(D21-C21)/C21*100</f>
         <v>-100</v>
       </c>
+      <c r="I21" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K21" s="4" t="n">
+        <v>554070</v>
+      </c>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4" t="n">
+        <f aca="false">(L21-K21)/K21*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="22">
       <c r="A22" s="4" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C22" s="4" t="n">
-        <v>239297</v>
+        <v>224094</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -601,16 +906,31 @@
         <f aca="false">(D22-C22)/C22*100</f>
         <v>-100</v>
       </c>
+      <c r="I22" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K22" s="4" t="n">
+        <v>224094</v>
+      </c>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4" t="n">
+        <f aca="false">(L22-K22)/K22*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="23">
       <c r="A23" s="4" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C23" s="4" t="n">
-        <v>336556</v>
+        <v>239297</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -618,73 +938,137 @@
         <f aca="false">(D23-C23)/C23*100</f>
         <v>-100</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="25">
-      <c r="A25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="I23" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K23" s="4" t="n">
+        <v>239297</v>
+      </c>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4" t="n">
+        <f aca="false">(L23-K23)/K23*100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="24">
+      <c r="A24" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="4" t="n">
+        <v>336556</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4" t="n">
+        <f aca="false">(D24-C24)/C24*100</f>
+        <v>-100</v>
+      </c>
+      <c r="I24" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K24" s="4" t="n">
+        <v>336556</v>
+      </c>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4" t="n">
+        <f aca="false">(L24-K24)/K24*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="26">
-      <c r="A26" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="A26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="I26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="27">
+      <c r="A27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="27">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="I27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="28">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="28">
-      <c r="A28" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="B28" s="4" t="s">
+      <c r="E28" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="4" t="n">
-        <v>2579</v>
-      </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4" t="n">
-        <f aca="false">(D28-C28)/C28*100</f>
-        <v>-100</v>
+      <c r="F28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N28" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="29">
       <c r="A29" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C29" s="4" t="n">
-        <v>10628</v>
+        <v>2579</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -692,16 +1076,31 @@
         <f aca="false">(D29-C29)/C29*100</f>
         <v>-100</v>
       </c>
+      <c r="I29" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K29" s="4" t="n">
+        <v>2579</v>
+      </c>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4" t="n">
+        <f aca="false">(L29-K29)/K29*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="30">
       <c r="A30" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C30" s="4" t="n">
-        <v>27686</v>
+        <v>10628</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -709,16 +1108,31 @@
         <f aca="false">(D30-C30)/C30*100</f>
         <v>-100</v>
       </c>
+      <c r="I30" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K30" s="4" t="n">
+        <v>10628</v>
+      </c>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4" t="n">
+        <f aca="false">(L30-K30)/K30*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="31">
       <c r="A31" s="4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C31" s="4" t="n">
-        <v>39</v>
+        <v>27686</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -726,16 +1140,31 @@
         <f aca="false">(D31-C31)/C31*100</f>
         <v>-100</v>
       </c>
+      <c r="I31" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K31" s="4" t="n">
+        <v>27686</v>
+      </c>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4" t="n">
+        <f aca="false">(L31-K31)/K31*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="32">
       <c r="A32" s="4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C32" s="4" t="n">
-        <v>25395</v>
+        <v>39</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -743,16 +1172,31 @@
         <f aca="false">(D32-C32)/C32*100</f>
         <v>-100</v>
       </c>
+      <c r="I32" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K32" s="4" t="n">
+        <v>39</v>
+      </c>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4" t="n">
+        <f aca="false">(L32-K32)/K32*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="33">
       <c r="A33" s="4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C33" s="4" t="n">
-        <v>22204</v>
+        <v>25395</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -760,16 +1204,31 @@
         <f aca="false">(D33-C33)/C33*100</f>
         <v>-100</v>
       </c>
+      <c r="I33" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K33" s="4" t="n">
+        <v>25395</v>
+      </c>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4" t="n">
+        <f aca="false">(L33-K33)/K33*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="34">
       <c r="A34" s="4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C34" s="4" t="n">
-        <v>28723</v>
+        <v>22204</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -777,16 +1236,31 @@
         <f aca="false">(D34-C34)/C34*100</f>
         <v>-100</v>
       </c>
+      <c r="I34" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K34" s="4" t="n">
+        <v>22204</v>
+      </c>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4" t="n">
+        <f aca="false">(L34-K34)/K34*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="35">
       <c r="A35" s="4" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C35" s="4" t="n">
-        <v>182566</v>
+        <v>28723</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -794,16 +1268,31 @@
         <f aca="false">(D35-C35)/C35*100</f>
         <v>-100</v>
       </c>
+      <c r="I35" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K35" s="4" t="n">
+        <v>28723</v>
+      </c>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4" t="n">
+        <f aca="false">(L35-K35)/K35*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="36">
       <c r="A36" s="4" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C36" s="4" t="n">
-        <v>22141</v>
+        <v>182566</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -811,16 +1300,31 @@
         <f aca="false">(D36-C36)/C36*100</f>
         <v>-100</v>
       </c>
+      <c r="I36" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K36" s="4" t="n">
+        <v>182566</v>
+      </c>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4" t="n">
+        <f aca="false">(L36-K36)/K36*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="37">
       <c r="A37" s="4" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C37" s="4" t="n">
-        <v>26130</v>
+        <v>22141</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -828,16 +1332,31 @@
         <f aca="false">(D37-C37)/C37*100</f>
         <v>-100</v>
       </c>
+      <c r="I37" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K37" s="4" t="n">
+        <v>22141</v>
+      </c>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4" t="n">
+        <f aca="false">(L37-K37)/K37*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="38">
       <c r="A38" s="4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C38" s="4" t="n">
-        <v>29437</v>
+        <v>26130</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -845,16 +1364,31 @@
         <f aca="false">(D38-C38)/C38*100</f>
         <v>-100</v>
       </c>
+      <c r="I38" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K38" s="4" t="n">
+        <v>26130</v>
+      </c>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4" t="n">
+        <f aca="false">(L38-K38)/K38*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="39">
       <c r="A39" s="4" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C39" s="4" t="n">
-        <v>20749</v>
+        <v>29437</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -862,16 +1396,31 @@
         <f aca="false">(D39-C39)/C39*100</f>
         <v>-100</v>
       </c>
+      <c r="I39" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K39" s="4" t="n">
+        <v>29437</v>
+      </c>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4" t="n">
+        <f aca="false">(L39-K39)/K39*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="40">
       <c r="A40" s="4" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C40" s="4" t="n">
-        <v>21294</v>
+        <v>20749</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -879,16 +1428,31 @@
         <f aca="false">(D40-C40)/C40*100</f>
         <v>-100</v>
       </c>
+      <c r="I40" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K40" s="4" t="n">
+        <v>20749</v>
+      </c>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4" t="n">
+        <f aca="false">(L40-K40)/K40*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="41">
       <c r="A41" s="4" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C41" s="4" t="n">
-        <v>23260728</v>
+        <v>21294</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
@@ -896,16 +1460,31 @@
         <f aca="false">(D41-C41)/C41*100</f>
         <v>-100</v>
       </c>
+      <c r="I41" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K41" s="4" t="n">
+        <v>21294</v>
+      </c>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4" t="n">
+        <f aca="false">(L41-K41)/K41*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="42">
       <c r="A42" s="4" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C42" s="4" t="n">
-        <v>378032</v>
+        <v>23260728</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
@@ -913,16 +1492,31 @@
         <f aca="false">(D42-C42)/C42*100</f>
         <v>-100</v>
       </c>
+      <c r="I42" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K42" s="4" t="n">
+        <v>23260728</v>
+      </c>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4" t="n">
+        <f aca="false">(L42-K42)/K42*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="43">
       <c r="A43" s="4" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C43" s="4" t="n">
-        <v>565040</v>
+        <v>378032</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
@@ -930,16 +1524,31 @@
         <f aca="false">(D43-C43)/C43*100</f>
         <v>-100</v>
       </c>
+      <c r="I43" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K43" s="4" t="n">
+        <v>378032</v>
+      </c>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4" t="n">
+        <f aca="false">(L43-K43)/K43*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="44">
       <c r="A44" s="4" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C44" s="4" t="n">
-        <v>554070</v>
+        <v>565040</v>
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
@@ -947,16 +1556,31 @@
         <f aca="false">(D44-C44)/C44*100</f>
         <v>-100</v>
       </c>
+      <c r="I44" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K44" s="4" t="n">
+        <v>565040</v>
+      </c>
+      <c r="L44" s="4"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="4" t="n">
+        <f aca="false">(L44-K44)/K44*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="45">
       <c r="A45" s="4" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C45" s="4" t="n">
-        <v>224094</v>
+        <v>554070</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
@@ -964,16 +1588,31 @@
         <f aca="false">(D45-C45)/C45*100</f>
         <v>-100</v>
       </c>
+      <c r="I45" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K45" s="4" t="n">
+        <v>554070</v>
+      </c>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4" t="n">
+        <f aca="false">(L45-K45)/K45*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="46">
       <c r="A46" s="4" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C46" s="4" t="n">
-        <v>239297</v>
+        <v>224094</v>
       </c>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
@@ -981,16 +1620,31 @@
         <f aca="false">(D46-C46)/C46*100</f>
         <v>-100</v>
       </c>
+      <c r="I46" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="J46" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K46" s="4" t="n">
+        <v>224094</v>
+      </c>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4" t="n">
+        <f aca="false">(L46-K46)/K46*100</f>
+        <v>-100</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="47">
       <c r="A47" s="4" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C47" s="4" t="n">
-        <v>336556</v>
+        <v>239297</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
@@ -998,19 +1652,78 @@
         <f aca="false">(D47-C47)/C47*100</f>
         <v>-100</v>
       </c>
+      <c r="I47" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K47" s="4" t="n">
+        <v>239297</v>
+      </c>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4" t="n">
+        <f aca="false">(L47-K47)/K47*100</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="48">
+      <c r="A48" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" s="4" t="n">
+        <v>336556</v>
+      </c>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4" t="n">
+        <f aca="false">(D48-C48)/C48*100</f>
+        <v>-100</v>
+      </c>
+      <c r="I48" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K48" s="4" t="n">
+        <v>336556</v>
+      </c>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4" t="n">
+        <f aca="false">(L48-K48)/K48*100</f>
+        <v>-100</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="22">
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="I26:N26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="K27:K28"/>
+    <mergeCell ref="L27:N27"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Ajout de mes résultats.
</commit_message>
<xml_diff>
--- a/Docs/doc_synthese/optimal.xlsx
+++ b/Docs/doc_synthese/optimal.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="42">
   <si>
     <t>Erwan</t>
   </si>
@@ -56,18 +56,30 @@
     <t>att48</t>
   </si>
   <si>
+    <t>0.675</t>
+  </si>
+  <si>
     <t>att532</t>
   </si>
   <si>
     <t>br17</t>
   </si>
   <si>
+    <t>0.171</t>
+  </si>
+  <si>
     <t>brazil58</t>
   </si>
   <si>
+    <t>0.309</t>
+  </si>
+  <si>
     <t>fl1577</t>
   </si>
   <si>
+    <t>1885.396</t>
+  </si>
+  <si>
     <t>fl3795</t>
   </si>
   <si>
@@ -83,6 +95,9 @@
     <t>kroB200</t>
   </si>
   <si>
+    <t>31.866</t>
+  </si>
+  <si>
     <t>kroC100</t>
   </si>
   <si>
@@ -114,6 +129,18 @@
   </si>
   <si>
     <t>88.559</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>945.651</t>
+  </si>
+  <si>
+    <t>20.38</t>
+  </si>
+  <si>
+    <t>55.152</t>
   </si>
 </sst>
 </file>
@@ -207,7 +234,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
@@ -221,6 +248,10 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -406,11 +437,15 @@
       <c r="K6" s="4" t="n">
         <v>10628</v>
       </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
+      <c r="L6" s="4" t="n">
+        <v>11196</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="N6" s="4" t="n">
         <f aca="false">(L6-K6)/K6*100</f>
-        <v>-100</v>
+        <v>5.3443733534061</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7">
@@ -418,7 +453,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="4" t="n">
         <v>27686</v>
@@ -433,16 +468,20 @@
         <v>2</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K7" s="4" t="n">
         <v>27686</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
+      <c r="L7" s="4" t="n">
+        <v>31778</v>
+      </c>
+      <c r="M7" s="5" t="n">
+        <v>10.94</v>
+      </c>
       <c r="N7" s="4" t="n">
         <f aca="false">(L7-K7)/K7*100</f>
-        <v>-100</v>
+        <v>14.7800332297912</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="8">
@@ -450,7 +489,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" s="4" t="n">
         <v>39</v>
@@ -465,16 +504,20 @@
         <v>3</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K8" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
+      <c r="L8" s="4" t="n">
+        <v>77</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="N8" s="4" t="n">
         <f aca="false">(L8-K8)/K8*100</f>
-        <v>-100</v>
+        <v>97.4358974358974</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
@@ -482,7 +525,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C9" s="4" t="n">
         <v>25395</v>
@@ -497,16 +540,20 @@
         <v>4</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K9" s="4" t="n">
         <v>25395</v>
       </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
+      <c r="L9" s="4" t="n">
+        <v>26573</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="N9" s="4" t="n">
         <f aca="false">(L9-K9)/K9*100</f>
-        <v>-100</v>
+        <v>4.63870840716677</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="10">
@@ -514,7 +561,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C10" s="4" t="n">
         <v>22204</v>
@@ -529,16 +576,20 @@
         <v>5</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K10" s="4" t="n">
         <v>22204</v>
       </c>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
+      <c r="L10" s="4" t="n">
+        <v>27788</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="N10" s="4" t="n">
         <f aca="false">(L10-K10)/K10*100</f>
-        <v>-100</v>
+        <v>25.1486218699333</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="11">
@@ -546,7 +597,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C11" s="4" t="n">
         <v>28723</v>
@@ -561,7 +612,7 @@
         <v>6</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="K11" s="4" t="n">
         <v>28723</v>
@@ -578,7 +629,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C12" s="4" t="n">
         <v>182566</v>
@@ -593,7 +644,7 @@
         <v>7</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="K12" s="4" t="n">
         <v>182566</v>
@@ -610,7 +661,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C13" s="4" t="n">
         <v>22141</v>
@@ -625,16 +676,20 @@
         <v>8</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="K13" s="4" t="n">
         <v>22141</v>
       </c>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
+      <c r="L13" s="4" t="n">
+        <v>24826</v>
+      </c>
+      <c r="M13" s="5" t="n">
+        <v>3.812</v>
+      </c>
       <c r="N13" s="4" t="n">
         <f aca="false">(L13-K13)/K13*100</f>
-        <v>-100</v>
+        <v>12.1268235400388</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="14">
@@ -642,7 +697,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C14" s="4" t="n">
         <v>26130</v>
@@ -657,16 +712,20 @@
         <v>9</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="K14" s="4" t="n">
         <v>26130</v>
       </c>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
+      <c r="L14" s="4" t="n">
+        <v>30609</v>
+      </c>
+      <c r="M14" s="5" t="n">
+        <v>12.711</v>
+      </c>
       <c r="N14" s="4" t="n">
         <f aca="false">(L14-K14)/K14*100</f>
-        <v>-100</v>
+        <v>17.1412169919633</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="15">
@@ -674,7 +733,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C15" s="4" t="n">
         <v>29437</v>
@@ -689,16 +748,20 @@
         <v>10</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="K15" s="4" t="n">
         <v>29437</v>
       </c>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
+      <c r="L15" s="4" t="n">
+        <v>31600</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="N15" s="4" t="n">
         <f aca="false">(L15-K15)/K15*100</f>
-        <v>-100</v>
+        <v>7.34789550565615</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="16">
@@ -706,7 +769,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C16" s="4" t="n">
         <v>20749</v>
@@ -721,16 +784,20 @@
         <v>11</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="K16" s="4" t="n">
         <v>20749</v>
       </c>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
+      <c r="L16" s="4" t="n">
+        <v>23250</v>
+      </c>
+      <c r="M16" s="4" t="n">
+        <v>5.44</v>
+      </c>
       <c r="N16" s="4" t="n">
         <f aca="false">(L16-K16)/K16*100</f>
-        <v>-100</v>
+        <v>12.0535929442383</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="17">
@@ -738,7 +805,7 @@
         <v>12</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C17" s="4" t="n">
         <v>21294</v>
@@ -753,16 +820,20 @@
         <v>12</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="K17" s="4" t="n">
         <v>21294</v>
       </c>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
+      <c r="L17" s="4" t="n">
+        <v>23642</v>
+      </c>
+      <c r="M17" s="4" t="n">
+        <v>4.084</v>
+      </c>
       <c r="N17" s="4" t="n">
         <f aca="false">(L17-K17)/K17*100</f>
-        <v>-100</v>
+        <v>11.0265802573495</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="18">
@@ -770,12 +841,12 @@
         <v>13</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C18" s="4" t="n">
         <v>23260728</v>
       </c>
-      <c r="D18" s="4"/>
+      <c r="D18" s="6"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4" t="n">
         <f aca="false">(D18-C18)/C18*100</f>
@@ -785,7 +856,7 @@
         <v>13</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="K18" s="4" t="n">
         <v>23260728</v>
@@ -802,7 +873,7 @@
         <v>14</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C19" s="4" t="n">
         <v>378032</v>
@@ -817,7 +888,7 @@
         <v>14</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K19" s="4" t="n">
         <v>378032</v>
@@ -834,7 +905,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C20" s="4" t="n">
         <v>565040</v>
@@ -849,7 +920,7 @@
         <v>15</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="K20" s="4" t="n">
         <v>565040</v>
@@ -866,7 +937,7 @@
         <v>16</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C21" s="4" t="n">
         <v>554070</v>
@@ -881,7 +952,7 @@
         <v>16</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="K21" s="4" t="n">
         <v>554070</v>
@@ -898,7 +969,7 @@
         <v>17</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C22" s="4" t="n">
         <v>224094</v>
@@ -913,7 +984,7 @@
         <v>17</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="K22" s="4" t="n">
         <v>224094</v>
@@ -930,7 +1001,7 @@
         <v>18</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C23" s="4" t="n">
         <v>239297</v>
@@ -945,7 +1016,7 @@
         <v>18</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="K23" s="4" t="n">
         <v>239297</v>
@@ -962,7 +1033,7 @@
         <v>19</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C24" s="4" t="n">
         <v>336556</v>
@@ -977,7 +1048,7 @@
         <v>19</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="K24" s="4" t="n">
         <v>336556</v>
@@ -991,7 +1062,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="26">
       <c r="A26" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -999,7 +1070,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="I26" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -1092,7 +1163,7 @@
         <v>2888</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="N29" s="4" t="n">
         <f aca="false">(L29-K29)/K29*100</f>
@@ -1109,11 +1180,15 @@
       <c r="C30" s="4" t="n">
         <v>10628</v>
       </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4" t="n">
+      <c r="D30" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30" s="4" t="e">
         <f aca="false">(D30-C30)/C30*100</f>
-        <v>-100</v>
+        <v>#VALUE!</v>
       </c>
       <c r="I30" s="4" t="n">
         <v>1</v>
@@ -1124,11 +1199,15 @@
       <c r="K30" s="4" t="n">
         <v>10628</v>
       </c>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
-      <c r="N30" s="4" t="n">
+      <c r="L30" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N30" s="4" t="e">
         <f aca="false">(L30-K30)/K30*100</f>
-        <v>-100</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="31">
@@ -1136,31 +1215,39 @@
         <v>2</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C31" s="4" t="n">
         <v>27686</v>
       </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4" t="n">
+      <c r="D31" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31" s="4" t="e">
         <f aca="false">(D31-C31)/C31*100</f>
-        <v>-100</v>
+        <v>#VALUE!</v>
       </c>
       <c r="I31" s="4" t="n">
         <v>2</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K31" s="4" t="n">
         <v>27686</v>
       </c>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4" t="n">
+      <c r="L31" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M31" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N31" s="4" t="e">
         <f aca="false">(L31-K31)/K31*100</f>
-        <v>-100</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="32">
@@ -1168,31 +1255,39 @@
         <v>3</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C32" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4" t="n">
+      <c r="D32" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F32" s="4" t="e">
         <f aca="false">(D32-C32)/C32*100</f>
-        <v>-100</v>
+        <v>#VALUE!</v>
       </c>
       <c r="I32" s="4" t="n">
         <v>3</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K32" s="4" t="n">
         <v>39</v>
       </c>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4" t="n">
+      <c r="L32" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M32" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N32" s="4" t="e">
         <f aca="false">(L32-K32)/K32*100</f>
-        <v>-100</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="33">
@@ -1200,31 +1295,39 @@
         <v>4</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C33" s="4" t="n">
         <v>25395</v>
       </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4" t="n">
+      <c r="D33" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F33" s="4" t="e">
         <f aca="false">(D33-C33)/C33*100</f>
-        <v>-100</v>
+        <v>#VALUE!</v>
       </c>
       <c r="I33" s="4" t="n">
         <v>4</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K33" s="4" t="n">
         <v>25395</v>
       </c>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4" t="n">
+      <c r="L33" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N33" s="4" t="e">
         <f aca="false">(L33-K33)/K33*100</f>
-        <v>-100</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="34">
@@ -1232,7 +1335,7 @@
         <v>5</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C34" s="4" t="n">
         <v>22204</v>
@@ -1247,16 +1350,20 @@
         <v>5</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="K34" s="4" t="n">
         <v>22204</v>
       </c>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
+      <c r="L34" s="4" t="n">
+        <v>27736</v>
+      </c>
+      <c r="M34" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="N34" s="4" t="n">
         <f aca="false">(L34-K34)/K34*100</f>
-        <v>-100</v>
+        <v>24.9144298324626</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="35">
@@ -1264,7 +1371,7 @@
         <v>6</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C35" s="4" t="n">
         <v>28723</v>
@@ -1279,7 +1386,7 @@
         <v>6</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="K35" s="4" t="n">
         <v>28723</v>
@@ -1296,7 +1403,7 @@
         <v>7</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C36" s="4" t="n">
         <v>182566</v>
@@ -1311,7 +1418,7 @@
         <v>7</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="K36" s="4" t="n">
         <v>182566</v>
@@ -1328,7 +1435,7 @@
         <v>8</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C37" s="4" t="n">
         <v>22141</v>
@@ -1343,16 +1450,20 @@
         <v>8</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="K37" s="4" t="n">
         <v>22141</v>
       </c>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
+      <c r="L37" s="4" t="n">
+        <v>24687</v>
+      </c>
+      <c r="M37" s="5" t="n">
+        <v>6.38</v>
+      </c>
       <c r="N37" s="4" t="n">
         <f aca="false">(L37-K37)/K37*100</f>
-        <v>-100</v>
+        <v>11.4990289508152</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="38">
@@ -1360,7 +1471,7 @@
         <v>9</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C38" s="4" t="n">
         <v>26130</v>
@@ -1375,16 +1486,20 @@
         <v>9</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="K38" s="4" t="n">
         <v>26130</v>
       </c>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
+      <c r="L38" s="4" t="n">
+        <v>31117</v>
+      </c>
+      <c r="M38" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="N38" s="4" t="n">
         <f aca="false">(L38-K38)/K38*100</f>
-        <v>-100</v>
+        <v>19.0853425181783</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="39">
@@ -1392,7 +1507,7 @@
         <v>10</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C39" s="4" t="n">
         <v>29437</v>
@@ -1407,16 +1522,20 @@
         <v>10</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="K39" s="4" t="n">
         <v>29437</v>
       </c>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
+      <c r="L39" s="4" t="n">
+        <v>31322</v>
+      </c>
+      <c r="M39" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="N39" s="4" t="n">
         <f aca="false">(L39-K39)/K39*100</f>
-        <v>-100</v>
+        <v>6.40350579203044</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="40">
@@ -1424,7 +1543,7 @@
         <v>11</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C40" s="4" t="n">
         <v>20749</v>
@@ -1439,16 +1558,20 @@
         <v>11</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="K40" s="4" t="n">
         <v>20749</v>
       </c>
-      <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
+      <c r="L40" s="4" t="n">
+        <v>23184</v>
+      </c>
+      <c r="M40" s="4" t="n">
+        <v>5.787</v>
+      </c>
       <c r="N40" s="4" t="n">
         <f aca="false">(L40-K40)/K40*100</f>
-        <v>-100</v>
+        <v>11.7355053255579</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="41">
@@ -1456,7 +1579,7 @@
         <v>12</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C41" s="4" t="n">
         <v>21294</v>
@@ -1471,16 +1594,20 @@
         <v>12</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="K41" s="4" t="n">
         <v>21294</v>
       </c>
-      <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
+      <c r="L41" s="4" t="n">
+        <v>23381</v>
+      </c>
+      <c r="M41" s="4" t="n">
+        <v>7.061</v>
+      </c>
       <c r="N41" s="4" t="n">
         <f aca="false">(L41-K41)/K41*100</f>
-        <v>-100</v>
+        <v>9.80088287780596</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="42">
@@ -1488,7 +1615,7 @@
         <v>13</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C42" s="4" t="n">
         <v>23260728</v>
@@ -1503,7 +1630,7 @@
         <v>13</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="K42" s="4" t="n">
         <v>23260728</v>
@@ -1520,7 +1647,7 @@
         <v>14</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C43" s="4" t="n">
         <v>378032</v>
@@ -1535,7 +1662,7 @@
         <v>14</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="K43" s="4" t="n">
         <v>378032</v>
@@ -1552,7 +1679,7 @@
         <v>15</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C44" s="4" t="n">
         <v>565040</v>
@@ -1567,7 +1694,7 @@
         <v>15</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="K44" s="4" t="n">
         <v>565040</v>
@@ -1584,7 +1711,7 @@
         <v>16</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C45" s="4" t="n">
         <v>554070</v>
@@ -1599,7 +1726,7 @@
         <v>16</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="K45" s="4" t="n">
         <v>554070</v>
@@ -1616,7 +1743,7 @@
         <v>17</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C46" s="4" t="n">
         <v>224094</v>
@@ -1631,7 +1758,7 @@
         <v>17</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="K46" s="4" t="n">
         <v>224094</v>
@@ -1648,7 +1775,7 @@
         <v>18</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C47" s="4" t="n">
         <v>239297</v>
@@ -1663,7 +1790,7 @@
         <v>18</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="K47" s="4" t="n">
         <v>239297</v>
@@ -1680,7 +1807,7 @@
         <v>19</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C48" s="4" t="n">
         <v>336556</v>
@@ -1695,7 +1822,7 @@
         <v>19</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="K48" s="4" t="n">
         <v>336556</v>

</xml_diff>

<commit_message>
Ajout de la synthèse.
</commit_message>
<xml_diff>
--- a/Docs/doc_synthese/optimal.xlsx
+++ b/Docs/doc_synthese/optimal.xlsx
@@ -240,7 +240,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
@@ -249,9 +249,6 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="2" fillId="0" fontId="0" numFmtId="164" xfId="0">
@@ -282,12 +279,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.54509803921569"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.8588235294118"/>
-    <col collapsed="false" hidden="false" max="13" min="7" style="0" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.8588235294118"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.56470588235294"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.9411764705882"/>
+    <col collapsed="false" hidden="false" max="13" min="7" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.9411764705882"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -482,7 +479,7 @@
       <c r="L7" s="4" t="n">
         <v>31778</v>
       </c>
-      <c r="M7" s="5" t="n">
+      <c r="M7" s="4" t="n">
         <v>10.94</v>
       </c>
       <c r="N7" s="4" t="n">
@@ -690,7 +687,7 @@
       <c r="L13" s="4" t="n">
         <v>24826</v>
       </c>
-      <c r="M13" s="5" t="n">
+      <c r="M13" s="4" t="n">
         <v>3.812</v>
       </c>
       <c r="N13" s="4" t="n">
@@ -726,7 +723,7 @@
       <c r="L14" s="4" t="n">
         <v>30609</v>
       </c>
-      <c r="M14" s="5" t="n">
+      <c r="M14" s="4" t="n">
         <v>12.711</v>
       </c>
       <c r="N14" s="4" t="n">
@@ -852,7 +849,7 @@
       <c r="C18" s="4" t="n">
         <v>23260728</v>
       </c>
-      <c r="D18" s="6"/>
+      <c r="D18" s="5"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4" t="n">
         <f aca="false">(D18-C18)/C18*100</f>
@@ -1468,7 +1465,7 @@
       <c r="L37" s="4" t="n">
         <v>24687</v>
       </c>
-      <c r="M37" s="5" t="n">
+      <c r="M37" s="4" t="n">
         <v>6.38</v>
       </c>
       <c r="N37" s="4" t="n">
@@ -1726,11 +1723,13 @@
       <c r="C45" s="4" t="n">
         <v>554070</v>
       </c>
-      <c r="D45" s="4"/>
+      <c r="D45" s="5" t="n">
+        <v>648800</v>
+      </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4" t="n">
         <f aca="false">(D45-C45)/C45*100</f>
-        <v>-100</v>
+        <v>17.0971176927103</v>
       </c>
       <c r="I45" s="4" t="n">
         <v>16</v>

</xml_diff>